<commit_message>
edit file excel download
</commit_message>
<xml_diff>
--- a/app/webroot/phpexcel/mau/mau_thanhtoan_thunhap_khac.xlsx
+++ b/app/webroot/phpexcel/mau/mau_thanhtoan_thunhap_khac.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/eoffice/app/webroot/phpexcel/mau/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D572D2-88F0-734F-AEA2-1FD65861E6AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3D0481-B873-4343-B849-7002E3DEB9FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Mã cán bộ</t>
   </si>
@@ -45,21 +45,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>NGUYỄN NGỌC VŨ</t>
-  </si>
-  <si>
-    <t>NGÔ VĂN DƯỠNG</t>
-  </si>
-  <si>
-    <t>LÊ QUANG SƠN</t>
-  </si>
-  <si>
-    <t>LÊ THÀNH BẮC</t>
-  </si>
-  <si>
-    <t>CAO XUÂN TUẤN</t>
-  </si>
-  <si>
     <t>BẢNG TỔNG HỢP THU NHẬP KHÁC</t>
   </si>
   <si>
@@ -88,6 +73,12 @@
   </si>
   <si>
     <t>Thực nhận</t>
+  </si>
+  <si>
+    <t>NGUYỄN NGỌC A</t>
+  </si>
+  <si>
+    <t>NGÔ VĂN B</t>
   </si>
 </sst>
 </file>
@@ -155,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -194,19 +185,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="dotted">
-        <color indexed="8"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="8"/>
@@ -253,6 +231,34 @@
       <top/>
       <bottom style="thin">
         <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="dotted">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -260,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -274,15 +280,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
@@ -310,17 +312,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,7 +622,7 @@
   <dimension ref="A2:W259"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -623,94 +641,94 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
+      <c r="I2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
     </row>
     <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
+      <c r="C4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>20</v>
+      <c r="M4" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2">
@@ -736,182 +754,84 @@
         <v>8</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <v>9</v>
       </c>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>103</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>9238000</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>1639000</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="8">
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7">
         <v>5</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>2284170</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="9">
+      <c r="K7" s="5"/>
+      <c r="L7" s="8">
         <v>7433332</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="8">
         <v>7433332</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>105</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="16">
+        <v>200</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="17">
+        <v>5</v>
+      </c>
+      <c r="D8" s="18">
+        <v>11383600</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1</v>
+      </c>
+      <c r="F8" s="18">
+        <v>1490000</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="17">
         <v>7</v>
       </c>
-      <c r="C8" s="8">
-        <v>5</v>
-      </c>
-      <c r="D8" s="9">
-        <v>11383600</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9">
-        <v>1490000</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8">
-        <v>7</v>
-      </c>
-      <c r="J8" s="9">
+      <c r="J8" s="18">
         <v>4248288</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="9">
+      <c r="K8" s="19"/>
+      <c r="L8" s="18">
         <v>17801312</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="18">
         <v>17801312</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>106</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="8">
-        <v>7</v>
-      </c>
-      <c r="D9" s="9">
-        <v>10310800</v>
-      </c>
-      <c r="E9" s="8">
-        <v>1</v>
-      </c>
-      <c r="F9" s="9">
-        <v>1490000</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="8">
-        <v>9</v>
-      </c>
-      <c r="J9" s="9">
-        <v>3540240</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="9">
-        <v>22940929</v>
-      </c>
-      <c r="M9" s="9">
-        <v>22940929</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>231</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8">
-        <v>8</v>
-      </c>
-      <c r="D10" s="9">
-        <v>10310800</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
-        <v>1490000</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="8">
-        <v>10</v>
-      </c>
-      <c r="J10" s="9">
-        <v>3422232</v>
-      </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="9">
-        <v>22163739</v>
-      </c>
-      <c r="M10" s="9">
-        <v>22163739</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>200</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="8">
-        <v>9</v>
-      </c>
-      <c r="D11" s="9">
-        <v>6436800</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F11" s="9">
-        <v>1192000</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="9">
-        <v>13138286</v>
-      </c>
-      <c r="M11" s="9">
-        <v>13138286</v>
-      </c>
-    </row>
+    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>